<commit_message>
modified currency converter api path, loginlogout api path, some changes in xml soccer test api
</commit_message>
<xml_diff>
--- a/TestData/Results.xlsx
+++ b/TestData/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="11">
   <si>
     <t>TestCase</t>
   </si>
@@ -41,6 +41,14 @@
   </si>
   <si>
     <t>Step02_AccessProp_CallClassMethod</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">java.lang.NullPointerException: Cannot invoke method getSheetAt() on null object
+error at line: 13
+</t>
   </si>
 </sst>
 </file>

</xml_diff>